<commit_message>
chore: Modificaciones en la BD de entrenamiento
</commit_message>
<xml_diff>
--- a/files/BD_HISTORIAS_CLINICAS_ENTRENAMIENTO.xlsx
+++ b/files/BD_HISTORIAS_CLINICAS_ENTRENAMIENTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8778beaa6210769/Escritorio/Github/UPC-Works/api-modelocombinado-aliviate/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{2F332284-391A-4B83-9EEC-BD41415BA7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{431992F0-BDDF-40C7-93F3-6A6975153E00}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{2F332284-391A-4B83-9EEC-BD41415BA7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C96FD6-D25A-4E7D-ABF4-581F93E603F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{93BB96C1-50B6-460C-8BBF-CB82EB3A8336}"/>
   </bookViews>
@@ -2242,10 +2242,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3913A69-7CCE-440C-99CB-A2CE04E78FBC}" name="Table1" displayName="Table1" ref="A1:CK95" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="A1:CK95" xr:uid="{B3913A69-7CCE-440C-99CB-A2CE04E78FBC}"/>
@@ -2641,10 +2637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57BBB6A-7852-481F-90C4-060FB3E6D97F}">
-  <dimension ref="A1:CK100"/>
+  <dimension ref="A1:CK95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV76" workbookViewId="0">
-      <selection activeCell="CJ78" sqref="CJ78"/>
+    <sheetView tabSelected="1" topLeftCell="AK76" workbookViewId="0">
+      <selection activeCell="AP99" sqref="AP99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28020,322 +28016,6 @@
         <v>127</v>
       </c>
     </row>
-    <row r="98" spans="1:89" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>1</v>
-      </c>
-      <c r="B98">
-        <v>2</v>
-      </c>
-      <c r="C98">
-        <v>3</v>
-      </c>
-      <c r="D98">
-        <v>4</v>
-      </c>
-      <c r="E98">
-        <v>5</v>
-      </c>
-      <c r="F98">
-        <v>6</v>
-      </c>
-      <c r="G98">
-        <v>7</v>
-      </c>
-      <c r="H98">
-        <v>8</v>
-      </c>
-      <c r="I98">
-        <v>9</v>
-      </c>
-      <c r="J98">
-        <v>10</v>
-      </c>
-      <c r="K98">
-        <v>11</v>
-      </c>
-      <c r="L98">
-        <v>12</v>
-      </c>
-      <c r="M98">
-        <v>13</v>
-      </c>
-      <c r="N98">
-        <v>14</v>
-      </c>
-      <c r="O98">
-        <v>15</v>
-      </c>
-      <c r="P98">
-        <v>16</v>
-      </c>
-      <c r="Q98">
-        <v>17</v>
-      </c>
-      <c r="R98">
-        <v>18</v>
-      </c>
-      <c r="S98">
-        <v>19</v>
-      </c>
-      <c r="T98">
-        <v>20</v>
-      </c>
-      <c r="U98">
-        <v>21</v>
-      </c>
-      <c r="V98">
-        <v>22</v>
-      </c>
-      <c r="W98">
-        <v>23</v>
-      </c>
-      <c r="X98">
-        <v>24</v>
-      </c>
-      <c r="Y98">
-        <v>25</v>
-      </c>
-      <c r="Z98">
-        <v>26</v>
-      </c>
-      <c r="AA98">
-        <v>27</v>
-      </c>
-      <c r="AB98">
-        <v>28</v>
-      </c>
-      <c r="AC98">
-        <v>29</v>
-      </c>
-      <c r="AD98">
-        <v>30</v>
-      </c>
-      <c r="AE98">
-        <v>31</v>
-      </c>
-      <c r="AF98">
-        <v>32</v>
-      </c>
-      <c r="AG98">
-        <v>33</v>
-      </c>
-      <c r="AH98">
-        <v>34</v>
-      </c>
-      <c r="AI98">
-        <v>35</v>
-      </c>
-      <c r="AJ98">
-        <v>36</v>
-      </c>
-      <c r="AK98">
-        <v>37</v>
-      </c>
-      <c r="AL98">
-        <v>38</v>
-      </c>
-      <c r="AM98">
-        <v>39</v>
-      </c>
-      <c r="AN98">
-        <v>40</v>
-      </c>
-      <c r="AO98">
-        <v>41</v>
-      </c>
-      <c r="AP98">
-        <v>42</v>
-      </c>
-      <c r="AQ98">
-        <v>43</v>
-      </c>
-      <c r="AR98">
-        <v>44</v>
-      </c>
-      <c r="AS98">
-        <v>45</v>
-      </c>
-      <c r="AT98">
-        <v>46</v>
-      </c>
-      <c r="AU98">
-        <v>47</v>
-      </c>
-      <c r="AV98">
-        <v>48</v>
-      </c>
-      <c r="AW98">
-        <v>49</v>
-      </c>
-      <c r="AX98">
-        <v>50</v>
-      </c>
-      <c r="AY98">
-        <v>51</v>
-      </c>
-      <c r="AZ98">
-        <v>52</v>
-      </c>
-      <c r="BA98">
-        <v>53</v>
-      </c>
-      <c r="BB98">
-        <v>54</v>
-      </c>
-      <c r="BC98">
-        <v>55</v>
-      </c>
-      <c r="BD98">
-        <v>56</v>
-      </c>
-      <c r="BE98">
-        <v>57</v>
-      </c>
-      <c r="BF98">
-        <v>58</v>
-      </c>
-      <c r="BG98">
-        <v>59</v>
-      </c>
-      <c r="BH98">
-        <v>60</v>
-      </c>
-      <c r="BI98">
-        <v>61</v>
-      </c>
-      <c r="BJ98">
-        <v>62</v>
-      </c>
-      <c r="BK98">
-        <v>63</v>
-      </c>
-      <c r="BL98">
-        <v>64</v>
-      </c>
-      <c r="BM98">
-        <v>65</v>
-      </c>
-      <c r="BN98">
-        <v>66</v>
-      </c>
-      <c r="BO98">
-        <v>67</v>
-      </c>
-      <c r="BP98">
-        <v>68</v>
-      </c>
-      <c r="BQ98">
-        <v>69</v>
-      </c>
-      <c r="BR98">
-        <v>70</v>
-      </c>
-      <c r="BS98">
-        <v>71</v>
-      </c>
-      <c r="BT98">
-        <v>72</v>
-      </c>
-      <c r="BU98">
-        <v>73</v>
-      </c>
-      <c r="BV98">
-        <v>74</v>
-      </c>
-      <c r="BW98">
-        <v>75</v>
-      </c>
-      <c r="BX98">
-        <v>76</v>
-      </c>
-      <c r="BY98">
-        <v>77</v>
-      </c>
-      <c r="BZ98">
-        <v>78</v>
-      </c>
-      <c r="CA98">
-        <v>79</v>
-      </c>
-      <c r="CB98">
-        <v>80</v>
-      </c>
-      <c r="CC98">
-        <v>81</v>
-      </c>
-      <c r="CD98">
-        <v>82</v>
-      </c>
-      <c r="CE98">
-        <v>83</v>
-      </c>
-      <c r="CF98">
-        <v>84</v>
-      </c>
-      <c r="CG98">
-        <v>85</v>
-      </c>
-      <c r="CH98">
-        <v>86</v>
-      </c>
-      <c r="CI98">
-        <v>87</v>
-      </c>
-      <c r="CJ98">
-        <v>88</v>
-      </c>
-      <c r="CK98">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="100" spans="1:89" x14ac:dyDescent="0.3">
-      <c r="BW100">
-        <v>1</v>
-      </c>
-      <c r="BX100">
-        <v>2</v>
-      </c>
-      <c r="BY100">
-        <v>3</v>
-      </c>
-      <c r="BZ100">
-        <v>4</v>
-      </c>
-      <c r="CA100">
-        <v>5</v>
-      </c>
-      <c r="CB100">
-        <v>6</v>
-      </c>
-      <c r="CC100">
-        <v>7</v>
-      </c>
-      <c r="CD100">
-        <v>8</v>
-      </c>
-      <c r="CE100">
-        <v>9</v>
-      </c>
-      <c r="CF100">
-        <v>10</v>
-      </c>
-      <c r="CG100">
-        <v>11</v>
-      </c>
-      <c r="CH100">
-        <v>12</v>
-      </c>
-      <c r="CI100">
-        <v>13</v>
-      </c>
-      <c r="CJ100">
-        <v>14</v>
-      </c>
-      <c r="CK100">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>